<commit_message>
Excel changes to work with the automator
</commit_message>
<xml_diff>
--- a/static/downloads/procfy_preenchido.xlsx
+++ b/static/downloads/procfy_preenchido.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -523,22 +523,22 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Despesas Variaveis</t>
+          <t>Transferência</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>31/10/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>TRANSF.REALIZADA PIX SICOOB-MESMA TIT. FAV.: MMG LOCACAO DE MAQUINAS LTDA Transferência Pix MMG LOCACAO DE MAQUINAS LTDA 44.388.803 0001-30</t>
         </is>
       </c>
       <c r="E2" s="5" t="n">
-        <v>7500</v>
+        <v>3040</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
@@ -576,25 +576,33 @@
       <c r="S2" t="inlineStr"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>31/10/2024</t>
+          <t>28/08/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
         </is>
       </c>
       <c r="E3" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
+        <v>3042.62</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>MMG LOCACAO DE MAQUINAS LTDA</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -627,25 +635,33 @@
       <c r="S3" t="inlineStr"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>31/10/2024</t>
+          <t>26/08/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>Contrato Natália Lopez</t>
         </is>
       </c>
       <c r="E4" s="5" t="n">
         <v>2000</v>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>MMG LOCACAO DE MAQUINAS LTDA</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -678,22 +694,30 @@
       <c r="S4" s="4" t="inlineStr"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>31/10/2024</t>
+          <t>26/08/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>asdasdasdasd</t>
+          <t>Contrato Natália Lopez</t>
         </is>
       </c>
       <c r="E5" s="5" t="n">
-        <v>4760.21</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
+        <v>1064.7</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>-</t>
@@ -729,22 +753,30 @@
       <c r="S5" t="inlineStr"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>22/08/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>qweqwe</t>
+          <t>Locação de equipamentos</t>
         </is>
       </c>
       <c r="E6" s="5" t="n">
-        <v>2200</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+        <v>1250</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>MMG LOCACAO DE MAQUINAS LTDA</t>
@@ -780,22 +812,30 @@
       <c r="S6" t="inlineStr"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>22/08/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PIX RECEBIDO - OUTRA IF Recebimento Pix RHTZ SERVICOS MEDICOS LTDA 52.305.548 0001-43</t>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
         </is>
       </c>
       <c r="E7" s="5" t="n">
-        <v>2197.5</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
+        <v>949.79</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>-</t>
@@ -831,25 +871,33 @@
       <c r="S7" t="inlineStr"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>22/08/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PIX EMITIDO OUTRA IF Pagamento Pix ***.276.298-**</t>
+          <t>CR ANTECIPAÇÃO VISA SIPAG_Ant._Visa</t>
         </is>
       </c>
       <c r="E8" s="5" t="n">
-        <v>7638</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+        <v>447.35</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Bruna Zavati Zavitoski</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -882,25 +930,33 @@
       <c r="S8" t="inlineStr"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>21/08/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>TRANSF.RECEBIDA - PIX SICOOB-MESMA TIT REM.: MMG LOCACAO DE MAQUINAS LTDA Transferência Pix MMG LOCACAO DE MAQUINAS LTDA 44.388.803 0001-30</t>
+          <t>Alimentação e hospedagem</t>
         </is>
       </c>
       <c r="E9" s="5" t="n">
-        <v>500</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+        <v>333</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>MMG LOCACAO DE MAQUINAS LTDA</t>
+          <t>ZOOP TECNOLOGIA &amp; INSTITUICAO DE PAGAMENTO S.A.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -933,25 +989,33 @@
       <c r="S9" t="inlineStr"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>21/08/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PIX RECEBIDO - OUTRA IF - MESMA TIT. Recebimento Pix MMG LOCACAO MAQUINAS LTDA 44.388.803 0001-30</t>
+          <t>Combustível</t>
         </is>
       </c>
       <c r="E10" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
+        <v>1000</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>MMG LOCACAO DE MAQUINAS LTDA</t>
+          <t>TICKET SOLUCOES HDFGT S/A</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -984,25 +1048,33 @@
       <c r="S10" t="inlineStr"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>21/08/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PIX EMITIDO OUTRA IF Pagamento Pix ***.295.638-**</t>
+          <t>Bruna</t>
         </is>
       </c>
       <c r="E11" s="5" t="n">
-        <v>2500</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
+        <v>10500</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Empréstimo</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Bruna Zavati Zavitoski</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1035,25 +1107,33 @@
       <c r="S11" t="inlineStr"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>21/08/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PIX EMITIDO OUTRA IF Pagamento Pix 20.729.204 0001-75</t>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
         </is>
       </c>
       <c r="E12" s="5" t="n">
-        <v>1620</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
+        <v>10750.25</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>LUME LASER - EQUIPAMENTOS PARA ESTETICA LTDA</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1086,22 +1166,30 @@
       <c r="S12" t="inlineStr"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>20/08/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>PIX RECEBIDO - OUTRA IF Recebimento Pix 52 866 790 KAMILLY KOWALCZYK 52.866.790 0001-96</t>
+          <t>Seguro de equipamento</t>
         </is>
       </c>
       <c r="E13" s="5" t="n">
-        <v>200</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+        <v>704.52</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>EASY SEGUROS MEDICOS LTDA</t>
@@ -1137,25 +1225,33 @@
       <c r="S13" t="inlineStr"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
+          <t>Alimentação e hospedagem</t>
         </is>
       </c>
       <c r="E14" s="5" t="n">
-        <v>8540.85</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ZOOP TECNOLOGIA &amp; INSTITUICAO DE PAGAMENTO S.A.</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1188,25 +1284,33 @@
       <c r="S14" t="inlineStr"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>PIX EMITIDO OUTRA IF Pagamento Pix 54.575.080 0001-32</t>
+          <t>Seguro Veicular</t>
         </is>
       </c>
       <c r="E15" s="5" t="n">
-        <v>2532.63</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+        <v>227.42</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ZOOP TECNOLOGIA &amp; INSTITUICAO DE PAGAMENTO S.A.</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1239,25 +1343,33 @@
       <c r="S15" t="inlineStr"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>TRANSF.RECEBIDA - PIX SICOOB-MESMA TIT REM.: MMG LOCACAO DE MAQUINAS LTDA Transferência Pix MMG LOCACAO DE MAQUINAS LTDA 44.388.803 0001-30</t>
+          <t>Manutenção de veículo</t>
         </is>
       </c>
       <c r="E16" s="5" t="n">
-        <v>1680</v>
-      </c>
-      <c r="F16" t="inlineStr"/>
+        <v>1070</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Manutenção de ativos</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>MMG LOCACAO DE MAQUINAS LTDA</t>
+          <t>MICHEL ALEXANDRE DE PAULA 39977974802</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1290,25 +1402,33 @@
       <c r="S16" t="inlineStr"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
+          <t>Bruna</t>
         </is>
       </c>
       <c r="E17" s="5" t="n">
-        <v>1424.68</v>
-      </c>
-      <c r="F17" t="inlineStr"/>
+        <v>12239.5</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Empréstimo</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Bruna Zavati Zavitoski</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1341,25 +1461,33 @@
       <c r="S17" t="inlineStr"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>DÉB.TIT.COMPE EFETIVADO</t>
+          <t>Pró-Labore - Guilherme</t>
         </is>
       </c>
       <c r="E18" s="5" t="n">
-        <v>7314.45</v>
-      </c>
-      <c r="F18" t="inlineStr"/>
+        <v>5131.42</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Guilherme Borelli</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1392,25 +1520,33 @@
       <c r="S18" t="inlineStr"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PIX RECEBIDO - OUTRA IF - MESMA TIT. Recebimento Pix MMG LOCACAO MAQUINAS LTDA 44.388.803 0001-30</t>
+          <t>CR ANTECIPAÇÃO VISA SIPAG_Ant._Visa</t>
         </is>
       </c>
       <c r="E19" s="5" t="n">
-        <v>3200</v>
-      </c>
-      <c r="F19" t="inlineStr"/>
+        <v>9854.440000000001</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>MMG LOCACAO DE MAQUINAS LTDA</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1443,10 +1579,14 @@
       <c r="S19" t="inlineStr"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1456,9 +1596,13 @@
         </is>
       </c>
       <c r="E20" s="5" t="n">
-        <v>3762.17</v>
-      </c>
-      <c r="F20" t="inlineStr"/>
+        <v>9854.440000000001</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>-</t>
@@ -1494,25 +1638,33 @@
       <c r="S20" t="inlineStr"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>15/08/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PIX RECEBIDO - OUTRA IF Recebimento Pix DERMA O C M LTDA - ME 18.706.583 0001-36</t>
+          <t>Locação de equipamentos</t>
         </is>
       </c>
       <c r="E21" s="5" t="n">
-        <v>396</v>
-      </c>
-      <c r="F21" t="inlineStr"/>
+        <v>2440</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>LUME LASER - EQUIPAMENTOS PARA ESTETICA LTDA</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1545,22 +1697,30 @@
       <c r="S21" t="inlineStr"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>15/08/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>SALDO BLOQUEADO ANTERIOR</t>
+          <t>Eugênio - Serviços evento</t>
         </is>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
+        <v>1900</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr">
         <is>
           <t>-</t>
@@ -1596,25 +1756,33 @@
       <c r="S22" t="inlineStr"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>14/08/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SALDO ANTERIOR</t>
+          <t>Renegociação boletos em atraso</t>
         </is>
       </c>
       <c r="E23" s="5" t="n">
-        <v>2.01</v>
-      </c>
-      <c r="F23" t="inlineStr"/>
+        <v>24377.8</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Compra de ativos</t>
+        </is>
+      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>PERSONALITE RECUPERACAO DE CREDITO LTDA</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1646,23 +1814,1009 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Despesas Variaveis</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>14/08/2024</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>3200</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Custos operacionais</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>13/08/2024</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Bruna</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>6880</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Bruna Zavati Zavitoski</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>13/08/2024</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>CR ANTECIPAÇÃO VISA SIPAG_Ant._Visa</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>19352.99</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13/08/2024</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>23293.38</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>12/08/2024</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Compras evento</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>1900</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>09/08/2024</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>CRED.TRANSF.CONTAS INTERCREDIS REM.: SUELLEN D. DA S. MENDES ESTETICA Transferência Pix SUELLEN D. DA S. MENDES ESTETICA 54.668.555 0001-35</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>497</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>SUELLEN D. DA S. MENDES ESTETICA</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>08/08/2024</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Pró-Labore - Thauana</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08/08/2024</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bruna</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>8063.51</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Empréstimo</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Bruna Zavati Zavitoski</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>08/08/2024</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
+        </is>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>8063.15</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>06/08/2024</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Ingresso evento</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>497</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Pessoas</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>05/08/2024</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Pró-Labore - Guilherme</t>
+        </is>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Despesas administrativas</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Guilherme Borelli</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>05/08/2024</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
+        </is>
+      </c>
+      <c r="E35" s="5" t="n">
+        <v>472.5</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>02/08/2024</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>PIX RECEBIDO - OUTRA IF Recebimento Pix CAROLINE ALMEIDA LEVORCI ***.523.890-**</t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Despesas Fixas</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>01/08/2024</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bradesco fiananciamento - Pixie</t>
+        </is>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>7809.48</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Compra de ativos</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>01/08/2024</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Ingresso evento</t>
+        </is>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>497</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>01/08/2024</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Ingresso evento</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>497</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>INFINITY COMPANY BY GG LTDA</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Recebimentos</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>01/08/2024</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>CR ANTECIPAÇÃO MASTERCARD SIPAG_Ant._Mastercard</t>
+        </is>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>2729.55</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Locação de equipamentos</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Preenchido Automaticamente</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Sicoob 2</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Indefinido</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+    </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1"/>

</xml_diff>